<commit_message>
temp finished merging of all sheetins including sum sheet
</commit_message>
<xml_diff>
--- a/nba/Part_2/TestFiles/2019_MEE_Even_A_19MEE444_a40c8852-1aa3-4153-bc21-beac8632da93.xlsx
+++ b/nba/Part_2/TestFiles/2019_MEE_Even_A_19MEE444_a40c8852-1aa3-4153-bc21-beac8632da93.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aseblr-my.sharepoint.com/personal/bl_en_u4aie20052_bl_students_amrita_edu/Documents/ASE/Projects/NBA/NBA_v3/dev_19.1/flux/nba/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aseblr-my.sharepoint.com/personal/bl_en_u4aie20052_bl_students_amrita_edu/Documents/ASE/Projects/NBA/NBA_v3/dev_19.1/flux/nba/Part_2/TestFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_ECA30ECFCA721965D6A61C1029AF1871AA80C564" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97A401FB-C624-48CE-87FB-431A730324C7}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="11_ECA30ECFCA721965D6A61C1029AF1871AA80C564" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7E0731E-7214-431E-B825-281BBB08F8B3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="27588" yWindow="2964" windowWidth="14400" windowHeight="7308" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A_Input_Details" sheetId="1" r:id="rId1"/>
@@ -1105,16 +1105,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1123,17 +1126,14 @@
     <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1556,6 +1556,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="A_Component_Details" displayName="A_Component_Details" ref="A22:B25">
   <autoFilter ref="A22:B25" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
@@ -1855,7 +1859,7 @@
   <dimension ref="A1:U29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2182,7 +2186,7 @@
         <v>24</v>
       </c>
       <c r="E11" s="17">
-        <v>86.8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
@@ -2193,7 +2197,7 @@
         <v>26</v>
       </c>
       <c r="E12" s="20">
-        <v>88.91</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
@@ -2206,7 +2210,7 @@
         <v>29</v>
       </c>
       <c r="E13" s="17">
-        <v>84.68</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
@@ -2221,7 +2225,7 @@
         <v>32</v>
       </c>
       <c r="E14" s="20">
-        <v>90.25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
@@ -2380,7 +2384,6 @@
       <c r="E29" s="3"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1"/>
   <mergeCells count="4">
     <mergeCell ref="D1:U1"/>
     <mergeCell ref="D9:E9"/>
@@ -2434,7 +2437,7 @@
   <dimension ref="A1:N64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:I5"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4858,7 +4861,6 @@
       <c r="C64" s="58"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1"/>
   <mergeCells count="7">
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="B9:I9"/>
@@ -6903,7 +6905,6 @@
       <c r="C64" s="58"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1"/>
   <mergeCells count="7">
     <mergeCell ref="B62:C62"/>
     <mergeCell ref="B64:C64"/>
@@ -10409,7 +10410,6 @@
       <c r="C64" s="58"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1"/>
   <mergeCells count="7">
     <mergeCell ref="B9:O9"/>
     <mergeCell ref="B1:O1"/>
@@ -13222,7 +13222,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1"/>
   <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="M1:P1"/>
@@ -13236,7 +13235,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -15115,7 +15116,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1"/>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="H1:K1"/>
@@ -15128,7 +15128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+    <sheetView topLeftCell="A74" workbookViewId="0">
       <selection activeCell="H87" sqref="H87"/>
     </sheetView>
   </sheetViews>
@@ -15154,20 +15154,20 @@
       <c r="B1" s="67" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="64"/>
+      <c r="C1" s="66"/>
       <c r="D1" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
     </row>
     <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="64"/>
+      <c r="A2" s="66"/>
       <c r="B2" s="67" t="s">
         <v>95</v>
       </c>
@@ -15177,32 +15177,32 @@
       <c r="D2" s="67" t="s">
         <v>97</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
       <c r="I2" s="67" t="s">
         <v>98</v>
       </c>
-      <c r="J2" s="64"/>
+      <c r="J2" s="66"/>
       <c r="K2" s="67" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="64"/>
-      <c r="B3" s="64"/>
-      <c r="C3" s="70" t="s">
+      <c r="A3" s="66"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="68" t="s">
         <v>100</v>
       </c>
       <c r="D3" s="67" t="s">
         <v>101</v>
       </c>
-      <c r="E3" s="64"/>
+      <c r="E3" s="66"/>
       <c r="F3" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="G3" s="64"/>
+      <c r="G3" s="66"/>
       <c r="H3" s="67" t="s">
         <v>103</v>
       </c>
@@ -15212,12 +15212,12 @@
       <c r="J3" s="67" t="s">
         <v>105</v>
       </c>
-      <c r="K3" s="64"/>
+      <c r="K3" s="66"/>
     </row>
     <row r="4" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A4" s="64"/>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
+      <c r="A4" s="66"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
       <c r="D4" s="42" t="s">
         <v>104</v>
       </c>
@@ -15230,9 +15230,9 @@
       <c r="G4" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
       <c r="K4" s="44" t="s">
         <v>107</v>
       </c>
@@ -15249,37 +15249,37 @@
         <f>A_Input_Details!E3</f>
         <v>3</v>
       </c>
-      <c r="D5" s="64">
+      <c r="D5" s="66">
         <f>IFERROR(A_Internal_Components!M58, 0)</f>
         <v>93.61702127659575</v>
       </c>
-      <c r="E5" s="66">
+      <c r="E5" s="64">
         <f>IF(AND(D5&gt;=0,D5&lt;40),1,IF(AND(D5&gt;=40,D5&lt;60),2,IF(AND(D5&gt;=60,D5&lt;=100),3,"0")))</f>
         <v>3</v>
       </c>
-      <c r="F5" s="64">
+      <c r="F5" s="66">
         <f>IFERROR(A_External_Components!H58, 0)</f>
         <v>76.59574468085107</v>
       </c>
-      <c r="G5" s="66">
+      <c r="G5" s="64">
         <f>IF(AND(F5&gt;=0,F5&lt;40),1,IF(AND(F5&gt;=40,F5&lt;60),2,IF(AND(F5&gt;=60,F5&lt;=100),3,"0")))</f>
         <v>3</v>
       </c>
-      <c r="H5" s="64">
+      <c r="H5" s="66">
         <f>E5*(A_Input_Details!B16/100)+G5*A_Input_Details!B15/100</f>
         <v>3</v>
       </c>
-      <c r="I5" s="66">
+      <c r="I5" s="64">
         <f>IF(A_Input_Details!E11&gt;0,A_Input_Details!E11,"0")</f>
-        <v>86.8</v>
-      </c>
-      <c r="J5" s="64">
+        <v>10</v>
+      </c>
+      <c r="J5" s="66">
         <f>IF(AND(I5&gt;=0,I5&lt;40),1,IF(AND(I5&gt;=40,I5&lt;60),2,IF(AND(I5&gt;=60,I5&lt;=100),3,"0")))</f>
-        <v>3</v>
-      </c>
-      <c r="K5" s="66">
+        <v>1</v>
+      </c>
+      <c r="K5" s="64">
         <f>(H5*(A_Input_Details!B17/100))+(J5*(A_Input_Details!B18/100))</f>
-        <v>3.0000000000000004</v>
+        <v>2.6000000000000005</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -15587,7 +15587,7 @@
       <c r="K21" s="65"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="70" t="s">
+      <c r="A22" s="68" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="43" t="str">
@@ -15598,37 +15598,37 @@
         <f>A_Input_Details!E4</f>
         <v>3</v>
       </c>
-      <c r="D22" s="64">
+      <c r="D22" s="66">
         <f>IFERROR(A_Internal_Components!N58, 0)</f>
         <v>95.744680851063833</v>
       </c>
-      <c r="E22" s="66">
+      <c r="E22" s="64">
         <f>IF(AND(D22&gt;=0,D22&lt;40),1,IF(AND(D22&gt;=40,D22&lt;60),2,IF(AND(D22&gt;=60,D22&lt;=100),3,"0")))</f>
         <v>3</v>
       </c>
-      <c r="F22" s="64">
+      <c r="F22" s="66">
         <f>IFERROR(A_External_Components!I58, 0)</f>
         <v>87.2340425531915</v>
       </c>
-      <c r="G22" s="66">
+      <c r="G22" s="64">
         <f>IF(AND(F22&gt;=0,F22&lt;40),1,IF(AND(F22&gt;=40,F22&lt;60),2,IF(AND(F22&gt;=60,F22&lt;=100),3,"0")))</f>
         <v>3</v>
       </c>
-      <c r="H22" s="64">
+      <c r="H22" s="66">
         <f>E22*(A_Input_Details!B16/100)+G22*A_Input_Details!B15/100</f>
         <v>3</v>
       </c>
-      <c r="I22" s="66">
+      <c r="I22" s="64">
         <f>IF(A_Input_Details!E12&gt;0,A_Input_Details!E12,"0")</f>
-        <v>88.91</v>
-      </c>
-      <c r="J22" s="64">
+        <v>10</v>
+      </c>
+      <c r="J22" s="66">
         <f>IF(AND(I22&gt;=0,I22&lt;40),1,IF(AND(I22&gt;=40,I22&lt;60),2,IF(AND(I22&gt;=60,I22&lt;=100),3,"0")))</f>
-        <v>3</v>
-      </c>
-      <c r="K22" s="66">
+        <v>1</v>
+      </c>
+      <c r="K22" s="64">
         <f>(H22*(A_Input_Details!B17/100))+(J22*(A_Input_Details!B18/100))</f>
-        <v>3.0000000000000004</v>
+        <v>2.6000000000000005</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -15947,37 +15947,37 @@
         <f>A_Input_Details!E5</f>
         <v>3</v>
       </c>
-      <c r="D39" s="64">
+      <c r="D39" s="66">
         <f>IFERROR(A_Internal_Components!O58, 0)</f>
         <v>100</v>
       </c>
-      <c r="E39" s="66">
+      <c r="E39" s="64">
         <f>IF(AND(D39&gt;=0,D39&lt;40),1,IF(AND(D39&gt;=40,D39&lt;60),2,IF(AND(D39&gt;=60,D39&lt;=100),3,"0")))</f>
         <v>3</v>
       </c>
-      <c r="F39" s="64">
+      <c r="F39" s="66">
         <f>IFERROR(A_External_Components!J58, 0)</f>
         <v>57.446808510638306</v>
       </c>
-      <c r="G39" s="66">
+      <c r="G39" s="64">
         <f>IF(AND(F39&gt;=0,F39&lt;40),1,IF(AND(F39&gt;=40,F39&lt;60),2,IF(AND(F39&gt;=60,F39&lt;=100),3,"0")))</f>
         <v>2</v>
       </c>
-      <c r="H39" s="64">
+      <c r="H39" s="66">
         <f>E39*(A_Input_Details!B16/100)+G39*A_Input_Details!B15/100</f>
         <v>2.5</v>
       </c>
-      <c r="I39" s="66">
+      <c r="I39" s="64">
         <f>IF(A_Input_Details!E13&gt;0,A_Input_Details!E13,"0")</f>
-        <v>84.68</v>
-      </c>
-      <c r="J39" s="64">
+        <v>10</v>
+      </c>
+      <c r="J39" s="66">
         <f>IF(AND(I39&gt;=0,I39&lt;40),1,IF(AND(I39&gt;=40,I39&lt;60),2,IF(AND(I39&gt;=60,I39&lt;=100),3,"0")))</f>
-        <v>3</v>
-      </c>
-      <c r="K39" s="66">
+        <v>1</v>
+      </c>
+      <c r="K39" s="64">
         <f>(H39*(A_Input_Details!B17/100))+(J39*(A_Input_Details!B18/100))</f>
-        <v>2.6</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
@@ -16285,7 +16285,7 @@
       <c r="K55" s="65"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A56" s="70" t="s">
+      <c r="A56" s="68" t="s">
         <v>32</v>
       </c>
       <c r="B56" s="43" t="str">
@@ -16296,37 +16296,37 @@
         <f>A_Input_Details!E6</f>
         <v>3</v>
       </c>
-      <c r="D56" s="64">
+      <c r="D56" s="66">
         <f>IFERROR(A_Internal_Components!P58, 0)</f>
         <v>100</v>
       </c>
-      <c r="E56" s="66">
+      <c r="E56" s="64">
         <f>IF(AND(D56&gt;=0,D56&lt;40),1,IF(AND(D56&gt;=40,D56&lt;60),2,IF(AND(D56&gt;=60,D56&lt;=100),3,"0")))</f>
         <v>3</v>
       </c>
-      <c r="F56" s="64">
+      <c r="F56" s="66">
         <f>IFERROR(A_External_Components!K58, 0)</f>
         <v>87.2340425531915</v>
       </c>
-      <c r="G56" s="66">
+      <c r="G56" s="64">
         <f>IF(AND(F56&gt;=0,F56&lt;40),1,IF(AND(F56&gt;=40,F56&lt;60),2,IF(AND(F56&gt;=60,F56&lt;=100),3,"0")))</f>
         <v>3</v>
       </c>
-      <c r="H56" s="64">
+      <c r="H56" s="66">
         <f>E56*(A_Input_Details!B16/100)+G56*A_Input_Details!B15/100</f>
         <v>3</v>
       </c>
-      <c r="I56" s="66">
+      <c r="I56" s="64">
         <f>IF(A_Input_Details!E14&gt;0,A_Input_Details!E14,"0")</f>
-        <v>90.25</v>
-      </c>
-      <c r="J56" s="64">
+        <v>10</v>
+      </c>
+      <c r="J56" s="66">
         <f>IF(AND(I56&gt;=0,I56&lt;40),1,IF(AND(I56&gt;=40,I56&lt;60),2,IF(AND(I56&gt;=60,I56&lt;=100),3,"0")))</f>
-        <v>3</v>
-      </c>
-      <c r="K56" s="66">
+        <v>1</v>
+      </c>
+      <c r="K56" s="64">
         <f>(H56*(A_Input_Details!B17/100))+(J56*(A_Input_Details!B18/100))</f>
-        <v>3.0000000000000004</v>
+        <v>2.6000000000000005</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
@@ -16634,7 +16634,7 @@
       <c r="K72" s="65"/>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="D76" s="68" t="s">
+      <c r="D76" s="69" t="s">
         <v>108</v>
       </c>
       <c r="E76" s="52"/>
@@ -16717,11 +16717,11 @@
       </c>
       <c r="E78" s="2">
         <f>C5*K5</f>
-        <v>9.0000000000000018</v>
+        <v>7.8000000000000016</v>
       </c>
       <c r="F78" s="2">
         <f>C6*K5</f>
-        <v>6.0000000000000009</v>
+        <v>5.2000000000000011</v>
       </c>
       <c r="G78" s="2">
         <f>C7*K5</f>
@@ -16757,15 +16757,15 @@
       </c>
       <c r="O78" s="2">
         <f>C15*K5</f>
-        <v>6.0000000000000009</v>
+        <v>5.2000000000000011</v>
       </c>
       <c r="P78" s="2">
         <f>C16*K5</f>
-        <v>6.0000000000000009</v>
+        <v>5.2000000000000011</v>
       </c>
       <c r="Q78" s="2">
         <f>C17*K5</f>
-        <v>9.0000000000000018</v>
+        <v>7.8000000000000016</v>
       </c>
       <c r="R78" s="2">
         <f>C18*K5</f>
@@ -16773,7 +16773,7 @@
       </c>
       <c r="S78" s="2">
         <f>C19*K5</f>
-        <v>3.0000000000000004</v>
+        <v>2.6000000000000005</v>
       </c>
       <c r="T78" s="2">
         <f>C20*K5</f>
@@ -16790,11 +16790,11 @@
       </c>
       <c r="E79" s="2">
         <f>C22*K22</f>
-        <v>9.0000000000000018</v>
+        <v>7.8000000000000016</v>
       </c>
       <c r="F79" s="2">
         <f>C23*K22</f>
-        <v>6.0000000000000009</v>
+        <v>5.2000000000000011</v>
       </c>
       <c r="G79" s="2">
         <f>C24*K22</f>
@@ -16830,15 +16830,15 @@
       </c>
       <c r="O79" s="2">
         <f>C32*K22</f>
-        <v>6.0000000000000009</v>
+        <v>5.2000000000000011</v>
       </c>
       <c r="P79" s="2">
         <f>C33*K22</f>
-        <v>6.0000000000000009</v>
+        <v>5.2000000000000011</v>
       </c>
       <c r="Q79" s="2">
         <f>C34*K22</f>
-        <v>9.0000000000000018</v>
+        <v>7.8000000000000016</v>
       </c>
       <c r="R79" s="2">
         <f>C35*K22</f>
@@ -16846,7 +16846,7 @@
       </c>
       <c r="S79" s="2">
         <f>C36*K22</f>
-        <v>3.0000000000000004</v>
+        <v>2.6000000000000005</v>
       </c>
       <c r="T79" s="2">
         <f>C37*K22</f>
@@ -16863,11 +16863,11 @@
       </c>
       <c r="E80" s="2">
         <f>C39*K39</f>
-        <v>7.8000000000000007</v>
+        <v>6.6000000000000005</v>
       </c>
       <c r="F80" s="2">
         <f>C40*K39</f>
-        <v>5.2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="G80" s="2">
         <f>C41*K39</f>
@@ -16903,15 +16903,15 @@
       </c>
       <c r="O80" s="2">
         <f>C49*K39</f>
-        <v>5.2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="P80" s="2">
         <f>C50*K39</f>
-        <v>5.2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="Q80" s="2">
         <f>C51*K39</f>
-        <v>7.8000000000000007</v>
+        <v>6.6000000000000005</v>
       </c>
       <c r="R80" s="2">
         <f>C52*K39</f>
@@ -16919,7 +16919,7 @@
       </c>
       <c r="S80" s="2">
         <f>C53*K39</f>
-        <v>2.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="T80" s="2">
         <f>C54*K39</f>
@@ -16936,11 +16936,11 @@
       </c>
       <c r="E81" s="2">
         <f>C56*K56</f>
-        <v>9.0000000000000018</v>
+        <v>7.8000000000000016</v>
       </c>
       <c r="F81" s="2">
         <f>C57*K56</f>
-        <v>6.0000000000000009</v>
+        <v>5.2000000000000011</v>
       </c>
       <c r="G81" s="2">
         <f>C58*K56</f>
@@ -16976,15 +16976,15 @@
       </c>
       <c r="O81" s="2">
         <f>C66*K56</f>
-        <v>6.0000000000000009</v>
+        <v>5.2000000000000011</v>
       </c>
       <c r="P81" s="2">
         <f>C67*K56</f>
-        <v>6.0000000000000009</v>
+        <v>5.2000000000000011</v>
       </c>
       <c r="Q81" s="2">
         <f>C68*K56</f>
-        <v>9.0000000000000018</v>
+        <v>7.8000000000000016</v>
       </c>
       <c r="R81" s="2">
         <f>C69*K56</f>
@@ -16992,7 +16992,7 @@
       </c>
       <c r="S81" s="2">
         <f>C70*K56</f>
-        <v>3.0000000000000004</v>
+        <v>2.6000000000000005</v>
       </c>
       <c r="T81" s="2">
         <f>C71*K56</f>
@@ -17016,7 +17016,7 @@
       <c r="D82" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="E82" s="69" t="s">
+      <c r="E82" s="70" t="s">
         <v>124</v>
       </c>
       <c r="F82" s="52"/>
@@ -17051,11 +17051,11 @@
       </c>
       <c r="E83" s="2">
         <f>IF(AND(SUM(E78:E81)&gt;0, SUM(A_Input_Details!E3:'A_Input_Details'!E6)&gt;0), SUM(E78:E81)/(SUM(A_Input_Details!E3:'A_Input_Details'!E6)), 0)</f>
-        <v>2.9000000000000004</v>
+        <v>2.5000000000000004</v>
       </c>
       <c r="F83" s="2">
         <f>IF(AND(SUM(F78:F81)&gt;0, SUM(A_Input_Details!F3:'A_Input_Details'!F6)&gt;0), SUM(F78:F81)/(SUM(A_Input_Details!F3:'A_Input_Details'!F6)), 0)</f>
-        <v>2.9000000000000004</v>
+        <v>2.5000000000000004</v>
       </c>
       <c r="G83" s="2">
         <f>IF(AND(SUM(G78:G81)&gt;0, SUM(A_Input_Details!G3:'A_Input_Details'!G6)&gt;0), SUM(G78:G81)/(SUM(A_Input_Details!G3:'A_Input_Details'!G6)), 0)</f>
@@ -17091,15 +17091,15 @@
       </c>
       <c r="O83" s="2">
         <f>IF(AND(SUM(O78:O81)&gt;0, SUM(A_Input_Details!O3:'A_Input_Details'!O6)&gt;0), SUM(O78:O81)/(SUM(A_Input_Details!O3:'A_Input_Details'!O6)), 0)</f>
-        <v>2.9000000000000004</v>
+        <v>2.5000000000000004</v>
       </c>
       <c r="P83" s="2">
         <f>IF(AND(SUM(P78:P81)&gt;0, SUM(A_Input_Details!P3:'A_Input_Details'!P6)&gt;0), SUM(P78:P81)/(SUM(A_Input_Details!P3:'A_Input_Details'!P6)), 0)</f>
-        <v>2.9000000000000004</v>
+        <v>2.5000000000000004</v>
       </c>
       <c r="Q83" s="2">
         <f>IF(AND(SUM(Q78:Q81)&gt;0, SUM(A_Input_Details!Q3:'A_Input_Details'!Q6)&gt;0), SUM(Q78:Q81)/(SUM(A_Input_Details!Q3:'A_Input_Details'!Q6)), 0)</f>
-        <v>2.9000000000000004</v>
+        <v>2.5000000000000004</v>
       </c>
       <c r="R83" s="2">
         <f>IF(AND(SUM(R78:R81)&gt;0, SUM(A_Input_Details!R3:'A_Input_Details'!R6)&gt;0), SUM(R78:R81)/(SUM(A_Input_Details!R3:'A_Input_Details'!R6)), 0)</f>
@@ -17107,7 +17107,7 @@
       </c>
       <c r="S83" s="2">
         <f>IF(AND(SUM(S78:S81)&gt;0, SUM(A_Input_Details!S3:'A_Input_Details'!S6)&gt;0), SUM(S78:S81)/(SUM(A_Input_Details!S3:'A_Input_Details'!S6)), 0)</f>
-        <v>2.9000000000000004</v>
+        <v>2.5000000000000004</v>
       </c>
       <c r="T83" s="2">
         <f>IF(AND(SUM(T78:T81)&gt;0, SUM(A_Input_Details!T3:'A_Input_Details'!T6)&gt;0), SUM(T78:T81)/(SUM(A_Input_Details!T3:'A_Input_Details'!T6)), 0)</f>
@@ -17119,7 +17119,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1"/>
   <mergeCells count="51">
     <mergeCell ref="E82:U82"/>
     <mergeCell ref="H39:H55"/>
@@ -17153,17 +17152,12 @@
     <mergeCell ref="H22:H38"/>
     <mergeCell ref="J22:J38"/>
     <mergeCell ref="D5:D21"/>
-    <mergeCell ref="E56:E72"/>
-    <mergeCell ref="D1:K1"/>
     <mergeCell ref="A39:A55"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="H5:H21"/>
     <mergeCell ref="A22:A38"/>
     <mergeCell ref="I39:I55"/>
-    <mergeCell ref="K39:K55"/>
-    <mergeCell ref="J56:J72"/>
     <mergeCell ref="C3:C4"/>
-    <mergeCell ref="G56:G72"/>
     <mergeCell ref="E22:E38"/>
     <mergeCell ref="G22:G38"/>
     <mergeCell ref="D39:D55"/>
@@ -17172,6 +17166,11 @@
     <mergeCell ref="E5:E21"/>
     <mergeCell ref="K5:K21"/>
     <mergeCell ref="J39:J55"/>
+    <mergeCell ref="E56:E72"/>
+    <mergeCell ref="D1:K1"/>
+    <mergeCell ref="K39:K55"/>
+    <mergeCell ref="J56:J72"/>
+    <mergeCell ref="G56:G72"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -17181,7 +17180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -17202,10 +17201,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="58"/>
-      <c r="D1" s="73" t="s">
+      <c r="D1" s="72" t="s">
         <v>125</v>
       </c>
-      <c r="E1" s="73" t="s">
+      <c r="E1" s="72" t="s">
         <v>126</v>
       </c>
       <c r="F1" s="71" t="s">
@@ -17325,7 +17324,7 @@
       <c r="B4" s="47">
         <v>2019</v>
       </c>
-      <c r="D4" s="72" t="s">
+      <c r="D4" s="73" t="s">
         <v>34</v>
       </c>
       <c r="E4" s="74" t="s">
@@ -17360,19 +17359,19 @@
       </c>
       <c r="M4" s="23">
         <f>A_Course_level_Attainment!I5</f>
-        <v>86.8</v>
+        <v>10</v>
       </c>
       <c r="N4" s="19">
         <f>A_Course_level_Attainment!J5</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O4" s="23">
         <f>(K4*(B17/100))+(M4*(B18/100))</f>
-        <v>85.445106382978736</v>
+        <v>70.085106382978736</v>
       </c>
       <c r="P4" s="19">
         <f>A_Course_level_Attainment!K5</f>
-        <v>3.0000000000000004</v>
+        <v>2.6000000000000005</v>
       </c>
       <c r="Q4" s="50">
         <f>B19</f>
@@ -17380,7 +17379,7 @@
       </c>
       <c r="R4" s="23" t="str">
         <f>IF(K4&gt;=M4,"Yes","No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -17421,19 +17420,19 @@
       </c>
       <c r="M5" s="23">
         <f>A_Course_level_Attainment!I22</f>
-        <v>88.91</v>
+        <v>10</v>
       </c>
       <c r="N5" s="19">
         <f>A_Course_level_Attainment!J22</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O5" s="23">
         <f>(K5*(B17/100))+(M5*(B18/100))</f>
-        <v>90.973489361702136</v>
+        <v>75.191489361702139</v>
       </c>
       <c r="P5" s="19">
         <f>A_Course_level_Attainment!K22</f>
-        <v>3.0000000000000004</v>
+        <v>2.6000000000000005</v>
       </c>
       <c r="Q5" s="50">
         <f>B19</f>
@@ -17482,19 +17481,19 @@
       </c>
       <c r="M6" s="23">
         <f>A_Course_level_Attainment!I39</f>
-        <v>84.68</v>
+        <v>10</v>
       </c>
       <c r="N6" s="19">
         <f>A_Course_level_Attainment!J39</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O6" s="23">
         <f>(K6*(B17/100))+(M6*(B18/100))</f>
-        <v>79.914723404255326</v>
+        <v>64.978723404255334</v>
       </c>
       <c r="P6" s="19">
         <f>A_Course_level_Attainment!K39</f>
-        <v>2.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="Q6" s="50">
         <f>B19</f>
@@ -17502,7 +17501,7 @@
       </c>
       <c r="R6" s="23" t="str">
         <f>IF(K6&gt;=M6,"Yes","No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
@@ -17543,19 +17542,19 @@
       </c>
       <c r="M7" s="23">
         <f>A_Course_level_Attainment!I56</f>
-        <v>90.25</v>
+        <v>10</v>
       </c>
       <c r="N7" s="19">
         <f>A_Course_level_Attainment!J56</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O7" s="23">
         <f>(K7*(B17/100))+(M7*(B18/100))</f>
-        <v>92.943617021276594</v>
+        <v>76.893617021276597</v>
       </c>
       <c r="P7" s="19">
         <f>A_Course_level_Attainment!K56</f>
-        <v>3.0000000000000004</v>
+        <v>2.6000000000000005</v>
       </c>
       <c r="Q7" s="50">
         <f>B19</f>
@@ -17659,7 +17658,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1"/>
   <mergeCells count="16">
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="M1:N2"/>

</xml_diff>